<commit_message>
Updated capacity factors from MERRA2 based to ERA5
</commit_message>
<xml_diff>
--- a/input_data/all_firm_case.xlsx
+++ b/input_data/all_firm_case.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliciawongel/Library/Group Containers/G69SCX94XU.duck/Library/Application Support/duck/Volumes.noindex/DPB-DGE Data Transfer Node/nobackup/scratch/awongel/clab_all_firm/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBDBF41-76FB-4443-A9AB-BA30268AB44E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A0B43B-1834-0342-9CB3-BD085387EF9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="1200" windowWidth="32860" windowHeight="19860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="case_input_intermodel_one_node_" sheetId="1" r:id="rId1"/>
@@ -279,12 +279,6 @@
     <t>geothermal</t>
   </si>
   <si>
-    <t>US_capacity_solar_25pctTop_unnormalized.csv</t>
-  </si>
-  <si>
-    <t>US_capacity_wind_25pctTop_unnormalized.csv</t>
-  </si>
-  <si>
     <t>US_demand_unnormalized.csv</t>
   </si>
   <si>
@@ -844,6 +838,12 @@
   </si>
   <si>
     <t>input_data/costs_2020.csv</t>
+  </si>
+  <si>
+    <t>20230922_US_mthd3_2010-2020_wind.csv</t>
+  </si>
+  <si>
+    <t>20230922_US_mthd3_2010-2020_solar.csv</t>
   </si>
 </sst>
 </file>
@@ -2195,8 +2195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="B42" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2521,18 +2521,18 @@
         <v>39</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B26" s="86" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G26" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -2548,7 +2548,7 @@
         <v>12</v>
       </c>
       <c r="B28" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -2556,7 +2556,7 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -2564,7 +2564,7 @@
         <v>36</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D30" t="s">
         <v>40</v>
@@ -2575,7 +2575,7 @@
         <v>37</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -2612,10 +2612,10 @@
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B36" s="73" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.2">
@@ -2623,7 +2623,7 @@
         <v>42</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D37" t="s">
         <v>46</v>
@@ -2655,19 +2655,19 @@
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C41" s="1"/>
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C42" s="1"/>
     </row>
@@ -2676,11 +2676,11 @@
         <v>64</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.2">
@@ -2696,16 +2696,16 @@
         <v>18</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G46" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="K46" t="s">
         <v>69</v>
       </c>
       <c r="P46" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.2">
@@ -2713,7 +2713,7 @@
         <v>62</v>
       </c>
       <c r="J47" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="R47" t="s">
         <v>61</v>
@@ -2800,7 +2800,7 @@
         <v>76</v>
       </c>
       <c r="P50" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="51" spans="1:26" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
@@ -2811,7 +2811,7 @@
         <v>21</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>22</v>
@@ -2820,13 +2820,13 @@
         <v>33</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I51" s="2" t="s">
         <v>43</v>
@@ -2844,7 +2844,7 @@
         <v>25</v>
       </c>
       <c r="Q51" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="R51" s="2" t="s">
         <v>26</v>
@@ -2859,7 +2859,7 @@
         <v>60</v>
       </c>
       <c r="V51" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X51" s="2" t="s">
         <v>27</v>
@@ -2874,14 +2874,14 @@
       </c>
       <c r="C52" s="21"/>
       <c r="D52" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E52" s="21"/>
       <c r="F52" s="21"/>
       <c r="G52" s="21"/>
       <c r="H52" s="21"/>
       <c r="I52" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J52" s="21"/>
       <c r="K52" s="21"/>
@@ -2911,37 +2911,37 @@
         <v>44</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
       <c r="I53" s="3" t="s">
-        <v>80</v>
+        <v>268</v>
       </c>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
       <c r="L53" s="54" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M53" s="3" t="str">
         <f>B43 &amp; "/time range/" &amp; B41</f>
         <v>€/time range/MW</v>
       </c>
       <c r="N53" s="90" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O53" s="3" t="str">
         <f xml:space="preserve"> B43 &amp; "/" &amp; B41 &amp; B40</f>
         <v>€/MWh</v>
       </c>
       <c r="P53" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q53" s="3"/>
       <c r="R53" s="3"/>
@@ -2958,37 +2958,37 @@
         <v>44</v>
       </c>
       <c r="B54" s="22" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C54" s="22"/>
       <c r="D54" s="22" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E54" s="22"/>
       <c r="F54" s="22"/>
       <c r="G54" s="22"/>
       <c r="H54" s="22"/>
       <c r="I54" s="22" t="s">
-        <v>81</v>
+        <v>267</v>
       </c>
       <c r="J54" s="22"/>
       <c r="K54" s="22"/>
       <c r="L54" s="55" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M54" s="22" t="str">
         <f>B43 &amp; "/time range/" &amp; B41</f>
         <v>€/time range/MW</v>
       </c>
       <c r="N54" s="91" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O54" s="22" t="str">
         <f xml:space="preserve"> B43 &amp; "/" &amp; B41 &amp; B40</f>
         <v>€/MWh</v>
       </c>
       <c r="P54" s="22" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q54" s="22"/>
       <c r="R54" s="22"/>
@@ -3005,13 +3005,13 @@
         <v>44</v>
       </c>
       <c r="B55" s="18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C55" s="18" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D55" s="18" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E55" s="18"/>
       <c r="F55" s="18"/>
@@ -3037,13 +3037,13 @@
         <v>€/MWh</v>
       </c>
       <c r="P55" s="18" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="Q55" s="18"/>
       <c r="R55" s="18"/>
       <c r="S55" s="18"/>
       <c r="T55" s="93" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U55" s="18"/>
       <c r="V55" s="17"/>
@@ -3056,19 +3056,19 @@
         <v>70</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D56" s="18" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E56" s="18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F56" s="18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G56" s="18"/>
       <c r="H56" s="18"/>
@@ -3090,7 +3090,7 @@
         <v>€/MWh</v>
       </c>
       <c r="P56" s="18" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q56" s="18"/>
       <c r="R56" s="18"/>
@@ -3100,7 +3100,7 @@
       </c>
       <c r="U56" s="18"/>
       <c r="V56" s="17" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="W56" s="18" t="str">
         <f>B42 &amp; "/" &amp;B41 &amp; B40</f>
@@ -3114,13 +3114,13 @@
         <v>44</v>
       </c>
       <c r="B57" s="76" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C57" s="76" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D57" s="76" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E57" s="76"/>
       <c r="F57" s="76"/>
@@ -3130,27 +3130,27 @@
       <c r="J57" s="76"/>
       <c r="K57" s="76"/>
       <c r="L57" s="77" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M57" s="76" t="str">
         <f>B43 &amp; "/time range/" &amp; B41</f>
         <v>€/time range/MW</v>
       </c>
       <c r="N57" s="77" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O57" s="76" t="str">
         <f xml:space="preserve"> B43 &amp; "/" &amp; B41 &amp; B40</f>
         <v>€/MWh</v>
       </c>
       <c r="P57" s="76" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q57" s="76"/>
       <c r="R57" s="76"/>
       <c r="S57" s="76"/>
       <c r="T57" s="77" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U57" s="76"/>
       <c r="V57" s="75"/>
@@ -3163,19 +3163,19 @@
         <v>70</v>
       </c>
       <c r="B58" s="76" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C58" s="76" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D58" s="76" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E58" s="76" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F58" s="76" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G58" s="76"/>
       <c r="H58" s="76"/>
@@ -3197,7 +3197,7 @@
         <v>€/MWh</v>
       </c>
       <c r="P58" s="76" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q58" s="76"/>
       <c r="R58" s="76"/>
@@ -3207,7 +3207,7 @@
       </c>
       <c r="U58" s="76"/>
       <c r="V58" s="75" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="W58" s="76" t="str">
         <f>B42 &amp; "/" &amp;B41 &amp; B40</f>
@@ -3221,13 +3221,13 @@
         <v>44</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E59" s="13"/>
       <c r="F59" s="13"/>
@@ -3253,7 +3253,7 @@
         <v>€/MWh</v>
       </c>
       <c r="P59" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="Q59" s="13"/>
       <c r="R59" s="13"/>
@@ -3270,19 +3270,19 @@
         <v>70</v>
       </c>
       <c r="B60" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="C60" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="D60" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="C60" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="D60" s="13" t="s">
-        <v>174</v>
-      </c>
       <c r="E60" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F60" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G60" s="13"/>
       <c r="H60" s="13"/>
@@ -3304,7 +3304,7 @@
         <v>€/MWh</v>
       </c>
       <c r="P60" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="Q60" s="13"/>
       <c r="R60" s="13"/>
@@ -3333,7 +3333,7 @@
         <v>79</v>
       </c>
       <c r="D61" s="24" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E61" s="24"/>
       <c r="F61" s="24"/>
@@ -3343,27 +3343,27 @@
       <c r="J61" s="24"/>
       <c r="K61" s="24"/>
       <c r="L61" s="57" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M61" s="24" t="str">
         <f>B43 &amp; "/time range/" &amp; B41</f>
         <v>€/time range/MW</v>
       </c>
       <c r="N61" s="94" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O61" s="24" t="str">
         <f xml:space="preserve"> B43 &amp; "/" &amp; B41 &amp; B40</f>
         <v>€/MWh</v>
       </c>
       <c r="P61" s="24" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q61" s="24"/>
       <c r="R61" s="24"/>
       <c r="S61" s="24"/>
       <c r="T61" s="57" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U61" s="24"/>
       <c r="V61" s="23"/>
@@ -3376,19 +3376,19 @@
         <v>70</v>
       </c>
       <c r="B62" s="24" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C62" s="24" t="s">
         <v>79</v>
       </c>
       <c r="D62" s="24" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E62" s="24" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F62" s="24" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G62" s="24"/>
       <c r="H62" s="24"/>
@@ -3410,7 +3410,7 @@
         <v>€/MWh</v>
       </c>
       <c r="P62" s="24" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q62" s="24"/>
       <c r="R62" s="24"/>
@@ -3420,7 +3420,7 @@
       </c>
       <c r="U62" s="24"/>
       <c r="V62" s="23" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="W62" s="24" t="str">
         <f>B42 &amp; "/" &amp;B41 &amp; B40</f>
@@ -3438,7 +3438,7 @@
       </c>
       <c r="C63" s="35"/>
       <c r="D63" s="35" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E63" s="35"/>
       <c r="F63" s="35"/>
@@ -3448,27 +3448,27 @@
       <c r="J63" s="35"/>
       <c r="K63" s="35"/>
       <c r="L63" s="78" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M63" s="35" t="str">
         <f>B43 &amp; "/time range/" &amp; B41</f>
         <v>€/time range/MW</v>
       </c>
       <c r="N63" s="95" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O63" s="35" t="str">
         <f xml:space="preserve"> B43 &amp; "/" &amp; B41 &amp; B40</f>
         <v>€/MWh</v>
       </c>
       <c r="P63" s="35" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q63" s="35"/>
       <c r="R63" s="35"/>
       <c r="S63" s="35"/>
       <c r="T63" s="95" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U63" s="35"/>
       <c r="V63" s="34"/>
@@ -3481,11 +3481,11 @@
         <v>44</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C64" s="15"/>
       <c r="D64" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E64" s="15"/>
       <c r="F64" s="15"/>
@@ -3495,27 +3495,27 @@
       <c r="J64" s="15"/>
       <c r="K64" s="15"/>
       <c r="L64" s="58" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M64" s="15" t="str">
         <f>B43 &amp; "/time range/" &amp; B41</f>
         <v>€/time range/MW</v>
       </c>
       <c r="N64" s="96" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O64" s="15" t="str">
         <f xml:space="preserve"> B43 &amp; "/" &amp; B41 &amp; B40</f>
         <v>€/MWh</v>
       </c>
       <c r="P64" s="15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q64" s="15"/>
       <c r="R64" s="15"/>
       <c r="S64" s="15"/>
       <c r="T64" s="58" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U64" s="15"/>
       <c r="V64" s="14"/>
@@ -3528,11 +3528,11 @@
         <v>71</v>
       </c>
       <c r="B65" s="62" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C65" s="62"/>
       <c r="D65" s="62" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E65" s="62"/>
       <c r="F65" s="62"/>
@@ -3555,7 +3555,7 @@
         <v>€/MWh</v>
       </c>
       <c r="P65" s="62" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="Q65" s="62">
         <v>-1</v>
@@ -3574,11 +3574,11 @@
         <v>71</v>
       </c>
       <c r="B66" s="64" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C66" s="64"/>
       <c r="D66" s="64" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E66" s="64"/>
       <c r="F66" s="64"/>
@@ -3601,7 +3601,7 @@
         <v>€/MWh</v>
       </c>
       <c r="P66" s="64" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="Q66" s="64"/>
       <c r="R66" s="64"/>
@@ -3618,11 +3618,11 @@
         <v>44</v>
       </c>
       <c r="B67" s="72" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C67" s="72"/>
       <c r="D67" s="72" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E67" s="72"/>
       <c r="F67" s="72"/>
@@ -3645,7 +3645,7 @@
         <v>€/MWh</v>
       </c>
       <c r="P67" s="72" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="Q67" s="72"/>
       <c r="R67" s="72"/>
@@ -3662,17 +3662,17 @@
         <v>70</v>
       </c>
       <c r="B68" s="70" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C68" s="70"/>
       <c r="D68" s="70" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E68" s="70" t="s">
         <v>78</v>
       </c>
       <c r="F68" s="70" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G68" s="70"/>
       <c r="H68" s="70"/>
@@ -3680,21 +3680,21 @@
       <c r="J68" s="70"/>
       <c r="K68" s="70"/>
       <c r="L68" s="83" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M68" s="70" t="str">
         <f>B43 &amp; "/time range/" &amp; B41</f>
         <v>€/time range/MW</v>
       </c>
       <c r="N68" s="103" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O68" s="70" t="str">
         <f xml:space="preserve"> B43 &amp; "/" &amp; B41 &amp; B40</f>
         <v>€/MWh</v>
       </c>
       <c r="P68" s="70" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q68" s="70"/>
       <c r="R68" s="70"/>
@@ -3702,7 +3702,7 @@
       <c r="T68" s="83"/>
       <c r="U68" s="70"/>
       <c r="V68" s="69" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="W68" s="70" t="str">
         <f xml:space="preserve"> B41 &amp; B40  &amp; "/" &amp;  B42</f>
@@ -3716,11 +3716,11 @@
         <v>71</v>
       </c>
       <c r="B69" s="33" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C69" s="33"/>
       <c r="D69" s="33" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E69" s="33"/>
       <c r="F69" s="33"/>
@@ -3742,7 +3742,7 @@
         <v>€/MWh</v>
       </c>
       <c r="P69" s="33" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="Q69" s="33"/>
       <c r="R69" s="33"/>
@@ -3759,7 +3759,7 @@
         <v>71</v>
       </c>
       <c r="B70" s="67" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C70" s="67"/>
       <c r="D70" s="67" t="s">
@@ -3773,18 +3773,18 @@
       <c r="J70" s="67"/>
       <c r="K70" s="67"/>
       <c r="L70" s="92" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M70" s="67" t="str">
         <f>B43 &amp; "/time range/" &amp; "CO2"</f>
         <v>€/time range/CO2</v>
       </c>
       <c r="N70" s="104" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O70" s="67"/>
       <c r="P70" s="67" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q70" s="67"/>
       <c r="R70" s="67"/>
@@ -3798,14 +3798,14 @@
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A71" s="25" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B71" s="26" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C71" s="26"/>
       <c r="D71" s="26" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E71" s="26"/>
       <c r="F71" s="26"/>
@@ -3830,7 +3830,7 @@
         <v>€/MWh</v>
       </c>
       <c r="P71" s="26" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q71" s="26"/>
       <c r="R71" s="26">
@@ -3851,16 +3851,16 @@
         <v>70</v>
       </c>
       <c r="B72" s="45" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C72" s="45" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D72" s="45" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E72" s="45" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F72" s="45"/>
       <c r="G72" s="45">
@@ -3871,15 +3871,15 @@
       <c r="J72" s="45"/>
       <c r="K72" s="45"/>
       <c r="L72" s="107" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M72" s="45"/>
       <c r="N72" s="107" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O72" s="45"/>
       <c r="P72" s="45" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q72" s="45"/>
       <c r="R72" s="45"/>
@@ -3896,13 +3896,13 @@
         <v>71</v>
       </c>
       <c r="B73" s="45" t="s">
+        <v>239</v>
+      </c>
+      <c r="C73" s="45" t="s">
+        <v>240</v>
+      </c>
+      <c r="D73" s="45" t="s">
         <v>241</v>
-      </c>
-      <c r="C73" s="45" t="s">
-        <v>242</v>
-      </c>
-      <c r="D73" s="45" t="s">
-        <v>243</v>
       </c>
       <c r="E73" s="45"/>
       <c r="F73" s="45"/>
@@ -3912,15 +3912,15 @@
       <c r="J73" s="45"/>
       <c r="K73" s="45"/>
       <c r="L73" s="107" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M73" s="45"/>
       <c r="N73" s="107" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O73" s="45"/>
       <c r="P73" s="45" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q73" s="45"/>
       <c r="R73" s="45"/>
@@ -3939,16 +3939,16 @@
         <v>70</v>
       </c>
       <c r="B74" s="72" t="s">
+        <v>242</v>
+      </c>
+      <c r="C74" s="72" t="s">
+        <v>243</v>
+      </c>
+      <c r="D74" s="72" t="s">
+        <v>86</v>
+      </c>
+      <c r="E74" s="72" t="s">
         <v>244</v>
-      </c>
-      <c r="C74" s="72" t="s">
-        <v>245</v>
-      </c>
-      <c r="D74" s="72" t="s">
-        <v>88</v>
-      </c>
-      <c r="E74" s="72" t="s">
-        <v>246</v>
       </c>
       <c r="F74" s="72"/>
       <c r="G74" s="72">
@@ -3959,15 +3959,15 @@
       <c r="J74" s="72"/>
       <c r="K74" s="72"/>
       <c r="L74" s="102" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M74" s="72"/>
       <c r="N74" s="102" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O74" s="72"/>
       <c r="P74" s="72" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q74" s="72"/>
       <c r="R74" s="72"/>
@@ -3984,13 +3984,13 @@
         <v>71</v>
       </c>
       <c r="B75" s="72" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C75" s="72" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D75" s="72" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E75" s="72"/>
       <c r="F75" s="72"/>
@@ -4000,15 +4000,15 @@
       <c r="J75" s="72"/>
       <c r="K75" s="72"/>
       <c r="L75" s="102" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M75" s="72"/>
       <c r="N75" s="102" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O75" s="72"/>
       <c r="P75" s="72" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q75" s="72"/>
       <c r="R75" s="72"/>
@@ -4027,16 +4027,16 @@
         <v>70</v>
       </c>
       <c r="B76" s="15" t="s">
+        <v>245</v>
+      </c>
+      <c r="C76" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="D76" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="E76" s="15" t="s">
         <v>247</v>
-      </c>
-      <c r="C76" s="15" t="s">
-        <v>248</v>
-      </c>
-      <c r="D76" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="E76" s="15" t="s">
-        <v>249</v>
       </c>
       <c r="F76" s="15"/>
       <c r="G76" s="15">
@@ -4047,15 +4047,15 @@
       <c r="J76" s="15"/>
       <c r="K76" s="15"/>
       <c r="L76" s="58" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M76" s="15"/>
       <c r="N76" s="58" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O76" s="15"/>
       <c r="P76" s="15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q76" s="15"/>
       <c r="R76" s="15"/>
@@ -4072,13 +4072,13 @@
         <v>71</v>
       </c>
       <c r="B77" s="15" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D77" s="15" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E77" s="15"/>
       <c r="F77" s="15"/>
@@ -4088,15 +4088,15 @@
       <c r="J77" s="15"/>
       <c r="K77" s="15"/>
       <c r="L77" s="58" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M77" s="15"/>
       <c r="N77" s="58" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O77" s="15"/>
       <c r="P77" s="15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q77" s="15"/>
       <c r="R77" s="15"/>
@@ -4115,16 +4115,16 @@
         <v>70</v>
       </c>
       <c r="B78" s="116" t="s">
+        <v>248</v>
+      </c>
+      <c r="C78" s="116" t="s">
+        <v>249</v>
+      </c>
+      <c r="D78" s="116" t="s">
+        <v>86</v>
+      </c>
+      <c r="E78" s="116" t="s">
         <v>250</v>
-      </c>
-      <c r="C78" s="116" t="s">
-        <v>251</v>
-      </c>
-      <c r="D78" s="116" t="s">
-        <v>88</v>
-      </c>
-      <c r="E78" s="116" t="s">
-        <v>252</v>
       </c>
       <c r="F78" s="116"/>
       <c r="G78" s="116">
@@ -4135,15 +4135,15 @@
       <c r="J78" s="116"/>
       <c r="K78" s="116"/>
       <c r="L78" s="117" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M78" s="116"/>
       <c r="N78" s="117" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O78" s="116"/>
       <c r="P78" s="116" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q78" s="116"/>
       <c r="R78" s="116"/>
@@ -4160,13 +4160,13 @@
         <v>71</v>
       </c>
       <c r="B79" s="116" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C79" s="116" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D79" s="116" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E79" s="116"/>
       <c r="F79" s="116"/>
@@ -4176,15 +4176,15 @@
       <c r="J79" s="116"/>
       <c r="K79" s="116"/>
       <c r="L79" s="117" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M79" s="116"/>
       <c r="N79" s="117" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O79" s="116"/>
       <c r="P79" s="116" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q79" s="116"/>
       <c r="R79" s="116"/>
@@ -4203,16 +4203,16 @@
         <v>70</v>
       </c>
       <c r="B80" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="C80" s="35" t="s">
         <v>190</v>
       </c>
-      <c r="C80" s="35" t="s">
-        <v>192</v>
-      </c>
       <c r="D80" s="35" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E80" s="35" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F80" s="35"/>
       <c r="G80" s="35">
@@ -4223,15 +4223,15 @@
       <c r="J80" s="35"/>
       <c r="K80" s="35"/>
       <c r="L80" s="95" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M80" s="35"/>
       <c r="N80" s="95" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O80" s="35"/>
       <c r="P80" s="35" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q80" s="35"/>
       <c r="R80" s="35"/>
@@ -4248,13 +4248,13 @@
         <v>71</v>
       </c>
       <c r="B81" s="35" t="s">
+        <v>189</v>
+      </c>
+      <c r="C81" s="35" t="s">
+        <v>190</v>
+      </c>
+      <c r="D81" s="35" t="s">
         <v>191</v>
-      </c>
-      <c r="C81" s="35" t="s">
-        <v>192</v>
-      </c>
-      <c r="D81" s="35" t="s">
-        <v>193</v>
       </c>
       <c r="E81" s="35"/>
       <c r="F81" s="35"/>
@@ -4264,15 +4264,15 @@
       <c r="J81" s="35"/>
       <c r="K81" s="35"/>
       <c r="L81" s="95" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M81" s="35"/>
       <c r="N81" s="95" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O81" s="35"/>
       <c r="P81" s="35" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q81" s="35"/>
       <c r="R81" s="35"/>
@@ -4291,16 +4291,16 @@
         <v>70</v>
       </c>
       <c r="B82" s="118" t="s">
+        <v>192</v>
+      </c>
+      <c r="C82" s="118" t="s">
         <v>194</v>
       </c>
-      <c r="C82" s="118" t="s">
-        <v>196</v>
-      </c>
       <c r="D82" s="118" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E82" s="118" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F82" s="118"/>
       <c r="G82" s="118">
@@ -4311,15 +4311,15 @@
       <c r="J82" s="118"/>
       <c r="K82" s="118"/>
       <c r="L82" s="119" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M82" s="118"/>
       <c r="N82" s="119" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O82" s="118"/>
       <c r="P82" s="118" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q82" s="118"/>
       <c r="R82" s="118"/>
@@ -4336,13 +4336,13 @@
         <v>71</v>
       </c>
       <c r="B83" s="118" t="s">
+        <v>193</v>
+      </c>
+      <c r="C83" s="118" t="s">
+        <v>194</v>
+      </c>
+      <c r="D83" s="118" t="s">
         <v>195</v>
-      </c>
-      <c r="C83" s="118" t="s">
-        <v>196</v>
-      </c>
-      <c r="D83" s="118" t="s">
-        <v>197</v>
       </c>
       <c r="E83" s="118"/>
       <c r="F83" s="118"/>
@@ -4352,15 +4352,15 @@
       <c r="J83" s="118"/>
       <c r="K83" s="118"/>
       <c r="L83" s="119" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M83" s="118"/>
       <c r="N83" s="119" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O83" s="118"/>
       <c r="P83" s="118" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q83" s="118"/>
       <c r="R83" s="118"/>
@@ -4379,16 +4379,16 @@
         <v>70</v>
       </c>
       <c r="B84" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E84" s="3" t="s">
         <v>253</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>255</v>
       </c>
       <c r="F84" s="3"/>
       <c r="G84" s="3">
@@ -4399,15 +4399,15 @@
       <c r="J84" s="3"/>
       <c r="K84" s="3"/>
       <c r="L84" s="54" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M84" s="3"/>
       <c r="N84" s="54" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O84" s="3"/>
       <c r="P84" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q84" s="3"/>
       <c r="R84" s="3"/>
@@ -4419,7 +4419,7 @@
       <c r="X84" s="3"/>
       <c r="Y84" s="3"/>
       <c r="Z84" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="85" spans="1:26" x14ac:dyDescent="0.2">
@@ -4427,13 +4427,13 @@
         <v>71</v>
       </c>
       <c r="B85" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C85" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="C85" s="3" t="s">
-        <v>256</v>
-      </c>
       <c r="D85" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
@@ -4443,15 +4443,15 @@
       <c r="J85" s="3"/>
       <c r="K85" s="3"/>
       <c r="L85" s="54" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M85" s="3"/>
       <c r="N85" s="54" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O85" s="3"/>
       <c r="P85" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q85" s="3"/>
       <c r="R85" s="3"/>
@@ -4465,7 +4465,7 @@
       <c r="X85" s="3"/>
       <c r="Y85" s="3"/>
       <c r="Z85" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="86" spans="1:26" x14ac:dyDescent="0.2">
@@ -4473,16 +4473,16 @@
         <v>70</v>
       </c>
       <c r="B86" s="45" t="s">
+        <v>255</v>
+      </c>
+      <c r="C86" s="45" t="s">
         <v>257</v>
       </c>
-      <c r="C86" s="45" t="s">
-        <v>259</v>
-      </c>
       <c r="D86" s="45" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E86" s="45" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F86" s="45"/>
       <c r="G86" s="45">
@@ -4493,15 +4493,15 @@
       <c r="J86" s="45"/>
       <c r="K86" s="45"/>
       <c r="L86" s="107" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M86" s="45"/>
       <c r="N86" s="107" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O86" s="45"/>
       <c r="P86" s="45" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q86" s="45"/>
       <c r="R86" s="45"/>
@@ -4513,7 +4513,7 @@
       <c r="X86" s="45"/>
       <c r="Y86" s="45"/>
       <c r="Z86" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="87" spans="1:26" x14ac:dyDescent="0.2">
@@ -4521,13 +4521,13 @@
         <v>71</v>
       </c>
       <c r="B87" s="45" t="s">
+        <v>256</v>
+      </c>
+      <c r="C87" s="45" t="s">
+        <v>257</v>
+      </c>
+      <c r="D87" s="45" t="s">
         <v>258</v>
-      </c>
-      <c r="C87" s="45" t="s">
-        <v>259</v>
-      </c>
-      <c r="D87" s="45" t="s">
-        <v>260</v>
       </c>
       <c r="E87" s="45"/>
       <c r="F87" s="45"/>
@@ -4537,15 +4537,15 @@
       <c r="J87" s="45"/>
       <c r="K87" s="45"/>
       <c r="L87" s="107" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M87" s="45"/>
       <c r="N87" s="107" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O87" s="45"/>
       <c r="P87" s="45" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q87" s="45"/>
       <c r="R87" s="45"/>
@@ -4559,7 +4559,7 @@
       <c r="X87" s="45"/>
       <c r="Y87" s="45"/>
       <c r="Z87" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="88" spans="1:26" x14ac:dyDescent="0.2">
@@ -4567,16 +4567,16 @@
         <v>70</v>
       </c>
       <c r="B88" s="35" t="s">
+        <v>181</v>
+      </c>
+      <c r="C88" s="35" t="s">
+        <v>184</v>
+      </c>
+      <c r="D88" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="E88" s="35" t="s">
         <v>183</v>
-      </c>
-      <c r="C88" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="D88" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="E88" s="35" t="s">
-        <v>185</v>
       </c>
       <c r="F88" s="35"/>
       <c r="G88" s="35">
@@ -4587,15 +4587,15 @@
       <c r="J88" s="35"/>
       <c r="K88" s="35"/>
       <c r="L88" s="95" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M88" s="35"/>
       <c r="N88" s="95" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O88" s="35"/>
       <c r="P88" s="35" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q88" s="35"/>
       <c r="R88" s="35"/>
@@ -4612,13 +4612,13 @@
         <v>71</v>
       </c>
       <c r="B89" s="35" t="s">
+        <v>182</v>
+      </c>
+      <c r="C89" s="35" t="s">
         <v>184</v>
       </c>
-      <c r="C89" s="35" t="s">
-        <v>186</v>
-      </c>
       <c r="D89" s="35" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E89" s="35"/>
       <c r="F89" s="35"/>
@@ -4628,15 +4628,15 @@
       <c r="J89" s="35"/>
       <c r="K89" s="35"/>
       <c r="L89" s="95" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M89" s="35"/>
       <c r="N89" s="95" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O89" s="35"/>
       <c r="P89" s="35" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q89" s="35"/>
       <c r="R89" s="35"/>
@@ -4655,16 +4655,16 @@
         <v>70</v>
       </c>
       <c r="B90" s="112" t="s">
+        <v>207</v>
+      </c>
+      <c r="C90" s="112" t="s">
         <v>209</v>
       </c>
-      <c r="C90" s="112" t="s">
-        <v>211</v>
-      </c>
       <c r="D90" s="112" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E90" s="112" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F90" s="112"/>
       <c r="G90" s="112">
@@ -4675,15 +4675,15 @@
       <c r="J90" s="112"/>
       <c r="K90" s="112"/>
       <c r="L90" s="113" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M90" s="112"/>
       <c r="N90" s="113" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O90" s="112"/>
       <c r="P90" s="112" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q90" s="112"/>
       <c r="R90" s="112"/>
@@ -4700,13 +4700,13 @@
         <v>71</v>
       </c>
       <c r="B91" s="112" t="s">
+        <v>208</v>
+      </c>
+      <c r="C91" s="112" t="s">
+        <v>209</v>
+      </c>
+      <c r="D91" s="112" t="s">
         <v>210</v>
-      </c>
-      <c r="C91" s="112" t="s">
-        <v>211</v>
-      </c>
-      <c r="D91" s="112" t="s">
-        <v>212</v>
       </c>
       <c r="E91" s="112"/>
       <c r="F91" s="112"/>
@@ -4716,15 +4716,15 @@
       <c r="J91" s="112"/>
       <c r="K91" s="112"/>
       <c r="L91" s="113" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M91" s="112"/>
       <c r="N91" s="113" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O91" s="112"/>
       <c r="P91" s="112" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q91" s="112"/>
       <c r="R91" s="112"/>
@@ -4743,16 +4743,16 @@
         <v>70</v>
       </c>
       <c r="B92" s="114" t="s">
+        <v>211</v>
+      </c>
+      <c r="C92" s="114" t="s">
         <v>213</v>
       </c>
-      <c r="C92" s="114" t="s">
-        <v>215</v>
-      </c>
       <c r="D92" s="114" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E92" s="114" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F92" s="114"/>
       <c r="G92" s="114">
@@ -4763,15 +4763,15 @@
       <c r="J92" s="114"/>
       <c r="K92" s="114"/>
       <c r="L92" s="115" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M92" s="114"/>
       <c r="N92" s="115" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O92" s="114"/>
       <c r="P92" s="114" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q92" s="114"/>
       <c r="R92" s="114"/>
@@ -4788,13 +4788,13 @@
         <v>71</v>
       </c>
       <c r="B93" s="114" t="s">
+        <v>212</v>
+      </c>
+      <c r="C93" s="114" t="s">
+        <v>213</v>
+      </c>
+      <c r="D93" s="114" t="s">
         <v>214</v>
-      </c>
-      <c r="C93" s="114" t="s">
-        <v>215</v>
-      </c>
-      <c r="D93" s="114" t="s">
-        <v>216</v>
       </c>
       <c r="E93" s="114"/>
       <c r="F93" s="114"/>
@@ -4804,15 +4804,15 @@
       <c r="J93" s="114"/>
       <c r="K93" s="114"/>
       <c r="L93" s="115" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M93" s="114"/>
       <c r="N93" s="115" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O93" s="114"/>
       <c r="P93" s="114" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q93" s="114"/>
       <c r="R93" s="114"/>
@@ -4831,16 +4831,16 @@
         <v>70</v>
       </c>
       <c r="B94" s="35" t="s">
+        <v>215</v>
+      </c>
+      <c r="C94" s="35" t="s">
         <v>217</v>
       </c>
-      <c r="C94" s="35" t="s">
-        <v>219</v>
-      </c>
       <c r="D94" s="35" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E94" s="35" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F94" s="35"/>
       <c r="G94" s="35">
@@ -4851,15 +4851,15 @@
       <c r="J94" s="35"/>
       <c r="K94" s="35"/>
       <c r="L94" s="95" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M94" s="35"/>
       <c r="N94" s="95" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O94" s="35"/>
       <c r="P94" s="35" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q94" s="35"/>
       <c r="R94" s="35"/>
@@ -4876,13 +4876,13 @@
         <v>71</v>
       </c>
       <c r="B95" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C95" s="35" t="s">
+        <v>217</v>
+      </c>
+      <c r="D95" s="35" t="s">
         <v>218</v>
-      </c>
-      <c r="C95" s="35" t="s">
-        <v>219</v>
-      </c>
-      <c r="D95" s="35" t="s">
-        <v>220</v>
       </c>
       <c r="E95" s="35"/>
       <c r="F95" s="35"/>
@@ -4892,15 +4892,15 @@
       <c r="J95" s="35"/>
       <c r="K95" s="35"/>
       <c r="L95" s="95" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M95" s="35"/>
       <c r="N95" s="95" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O95" s="35"/>
       <c r="P95" s="35" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q95" s="35"/>
       <c r="R95" s="35"/>
@@ -4919,16 +4919,16 @@
         <v>70</v>
       </c>
       <c r="B96" s="30" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C96" s="30" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D96" s="30" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E96" s="30" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F96" s="30"/>
       <c r="G96" s="30">
@@ -4939,21 +4939,21 @@
       <c r="J96" s="30"/>
       <c r="K96" s="30"/>
       <c r="L96" s="31" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M96" s="30" t="str">
         <f>B43 &amp; "/time range/" &amp; B41</f>
         <v>€/time range/MW</v>
       </c>
       <c r="N96" s="98" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O96" s="30" t="str">
         <f xml:space="preserve"> B43 &amp; "/" &amp; B41 &amp; B40</f>
         <v>€/MWh</v>
       </c>
       <c r="P96" s="30" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q96" s="30"/>
       <c r="R96" s="30"/>
@@ -4970,13 +4970,13 @@
         <v>71</v>
       </c>
       <c r="B97" s="30" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C97" s="30" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D97" s="30" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E97" s="30"/>
       <c r="F97" s="30"/>
@@ -4986,21 +4986,21 @@
       <c r="J97" s="30"/>
       <c r="K97" s="30"/>
       <c r="L97" s="31" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M97" s="30" t="str">
         <f>B43 &amp; "/time range/" &amp; B41 &amp; B40</f>
         <v>€/time range/MWh</v>
       </c>
       <c r="N97" s="99" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O97" s="30" t="str">
         <f xml:space="preserve"> B43 &amp; "/" &amp; B41 &amp; B40</f>
         <v>€/MWh</v>
       </c>
       <c r="P97" s="30" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q97" s="30"/>
       <c r="R97" s="30"/>
@@ -5022,10 +5022,10 @@
         <v>32</v>
       </c>
       <c r="C98" s="28" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D98" s="28" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E98" s="28" t="s">
         <v>34</v>
@@ -5037,7 +5037,7 @@
       <c r="J98" s="28"/>
       <c r="K98" s="28"/>
       <c r="L98" s="60" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M98" s="28" t="str">
         <f>B43 &amp; "/time range/" &amp; B41</f>
@@ -5051,13 +5051,13 @@
         <v>€/MWh</v>
       </c>
       <c r="P98" s="28" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q98" s="28"/>
       <c r="R98" s="28"/>
       <c r="S98" s="28"/>
       <c r="T98" s="60" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U98" s="28"/>
       <c r="V98" s="27"/>
@@ -5070,10 +5070,10 @@
         <v>71</v>
       </c>
       <c r="B99" s="28" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C99" s="28" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D99" s="28" t="s">
         <v>34</v>
@@ -5086,21 +5086,21 @@
       <c r="J99" s="28"/>
       <c r="K99" s="28"/>
       <c r="L99" s="60" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M99" s="28" t="str">
         <f>B43 &amp; "/time range/" &amp; B41 &amp; B40</f>
         <v>€/time range/MWh</v>
       </c>
       <c r="N99" s="97" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O99" s="28" t="str">
         <f xml:space="preserve"> B43 &amp; "/" &amp; B41 &amp; B40</f>
         <v>€/MWh</v>
       </c>
       <c r="P99" s="28" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q99" s="28"/>
       <c r="R99" s="28"/>
@@ -5108,7 +5108,7 @@
         <v>1</v>
       </c>
       <c r="T99" s="60" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U99" s="28"/>
       <c r="V99" s="27"/>
@@ -5123,16 +5123,16 @@
         <v>70</v>
       </c>
       <c r="B100" s="28" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C100" s="28" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D100" s="28" t="s">
         <v>34</v>
       </c>
       <c r="E100" s="28" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F100" s="28"/>
       <c r="G100" s="28"/>
@@ -5141,7 +5141,7 @@
       <c r="J100" s="28"/>
       <c r="K100" s="28"/>
       <c r="L100" s="60" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M100" s="28" t="str">
         <f>B43 &amp; "/time range/" &amp; B41</f>
@@ -5155,13 +5155,13 @@
         <v>€/MWh</v>
       </c>
       <c r="P100" s="28" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q100" s="28"/>
       <c r="R100" s="28"/>
       <c r="S100" s="28"/>
       <c r="T100" s="60" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U100" s="28"/>
       <c r="V100" s="27"/>
@@ -5174,16 +5174,16 @@
         <v>70</v>
       </c>
       <c r="B101" s="110" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C101" s="110" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D101" s="110" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E101" s="110" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F101" s="110"/>
       <c r="G101" s="110"/>
@@ -5192,15 +5192,15 @@
       <c r="J101" s="110"/>
       <c r="K101" s="110"/>
       <c r="L101" s="111" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M101" s="110"/>
       <c r="N101" s="111" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O101" s="110"/>
       <c r="P101" s="110" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q101" s="110"/>
       <c r="R101" s="110"/>
@@ -5217,13 +5217,13 @@
         <v>71</v>
       </c>
       <c r="B102" s="110" t="s">
+        <v>202</v>
+      </c>
+      <c r="C102" s="110" t="s">
         <v>204</v>
       </c>
-      <c r="C102" s="110" t="s">
-        <v>206</v>
-      </c>
       <c r="D102" s="110" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E102" s="110"/>
       <c r="F102" s="110"/>
@@ -5233,15 +5233,15 @@
       <c r="J102" s="110"/>
       <c r="K102" s="110"/>
       <c r="L102" s="111" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M102" s="110"/>
       <c r="N102" s="111" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O102" s="110"/>
       <c r="P102" s="110" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q102" s="110"/>
       <c r="R102" s="110"/>
@@ -5260,16 +5260,16 @@
         <v>70</v>
       </c>
       <c r="B103" s="110" t="s">
+        <v>203</v>
+      </c>
+      <c r="C103" s="110" t="s">
+        <v>204</v>
+      </c>
+      <c r="D103" s="110" t="s">
         <v>205</v>
       </c>
-      <c r="C103" s="110" t="s">
-        <v>206</v>
-      </c>
-      <c r="D103" s="110" t="s">
-        <v>207</v>
-      </c>
       <c r="E103" s="110" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F103" s="110"/>
       <c r="G103" s="110"/>
@@ -5278,15 +5278,15 @@
       <c r="J103" s="110"/>
       <c r="K103" s="110"/>
       <c r="L103" s="111" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M103" s="110"/>
       <c r="N103" s="111" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O103" s="110"/>
       <c r="P103" s="110" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q103" s="110"/>
       <c r="R103" s="110"/>
@@ -5303,16 +5303,16 @@
         <v>70</v>
       </c>
       <c r="B104" s="108" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C104" s="108" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D104" s="108" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E104" s="108" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F104" s="108"/>
       <c r="G104" s="108"/>
@@ -5321,15 +5321,15 @@
       <c r="J104" s="108"/>
       <c r="K104" s="108"/>
       <c r="L104" s="109" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M104" s="108"/>
       <c r="N104" s="109" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O104" s="108"/>
       <c r="P104" s="108" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q104" s="108"/>
       <c r="R104" s="108"/>
@@ -5346,13 +5346,13 @@
         <v>71</v>
       </c>
       <c r="B105" s="108" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C105" s="108" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D105" s="108" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E105" s="108"/>
       <c r="F105" s="108"/>
@@ -5362,15 +5362,15 @@
       <c r="J105" s="108"/>
       <c r="K105" s="108"/>
       <c r="L105" s="109" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M105" s="108"/>
       <c r="N105" s="109" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O105" s="108"/>
       <c r="P105" s="108" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q105" s="108"/>
       <c r="R105" s="108"/>
@@ -5389,16 +5389,16 @@
         <v>70</v>
       </c>
       <c r="B106" s="108" t="s">
+        <v>220</v>
+      </c>
+      <c r="C106" s="108" t="s">
+        <v>226</v>
+      </c>
+      <c r="D106" s="108" t="s">
         <v>222</v>
       </c>
-      <c r="C106" s="108" t="s">
-        <v>228</v>
-      </c>
-      <c r="D106" s="108" t="s">
-        <v>224</v>
-      </c>
       <c r="E106" s="108" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F106" s="108"/>
       <c r="G106" s="108"/>
@@ -5407,15 +5407,15 @@
       <c r="J106" s="108"/>
       <c r="K106" s="108"/>
       <c r="L106" s="109" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M106" s="108"/>
       <c r="N106" s="109" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O106" s="108"/>
       <c r="P106" s="108" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q106" s="108"/>
       <c r="R106" s="108"/>
@@ -5432,16 +5432,16 @@
         <v>70</v>
       </c>
       <c r="B107" s="45" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C107" s="45" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D107" s="45" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E107" s="45" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F107" s="45"/>
       <c r="G107" s="45"/>
@@ -5450,15 +5450,15 @@
       <c r="J107" s="45"/>
       <c r="K107" s="45"/>
       <c r="L107" s="107" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M107" s="45"/>
       <c r="N107" s="107" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O107" s="45"/>
       <c r="P107" s="45" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q107" s="45"/>
       <c r="R107" s="45"/>
@@ -5475,13 +5475,13 @@
         <v>71</v>
       </c>
       <c r="B108" s="45" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C108" s="45" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D108" s="45" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E108" s="45"/>
       <c r="F108" s="45"/>
@@ -5491,15 +5491,15 @@
       <c r="J108" s="45"/>
       <c r="K108" s="45"/>
       <c r="L108" s="107" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M108" s="45"/>
       <c r="N108" s="107" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O108" s="45"/>
       <c r="P108" s="45" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q108" s="45"/>
       <c r="R108" s="45"/>
@@ -5518,16 +5518,16 @@
         <v>70</v>
       </c>
       <c r="B109" s="45" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C109" s="45" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D109" s="45" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E109" s="45" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F109" s="45"/>
       <c r="G109" s="45"/>
@@ -5536,15 +5536,15 @@
       <c r="J109" s="45"/>
       <c r="K109" s="45"/>
       <c r="L109" s="107" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M109" s="45"/>
       <c r="N109" s="107" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O109" s="45"/>
       <c r="P109" s="45" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q109" s="45"/>
       <c r="R109" s="45"/>
@@ -5561,16 +5561,16 @@
         <v>70</v>
       </c>
       <c r="B110" s="70" t="s">
+        <v>231</v>
+      </c>
+      <c r="C110" s="70" t="s">
+        <v>232</v>
+      </c>
+      <c r="D110" s="70" t="s">
+        <v>86</v>
+      </c>
+      <c r="E110" s="70" t="s">
         <v>233</v>
-      </c>
-      <c r="C110" s="70" t="s">
-        <v>234</v>
-      </c>
-      <c r="D110" s="70" t="s">
-        <v>88</v>
-      </c>
-      <c r="E110" s="70" t="s">
-        <v>235</v>
       </c>
       <c r="F110" s="70"/>
       <c r="G110" s="70"/>
@@ -5579,15 +5579,15 @@
       <c r="J110" s="70"/>
       <c r="K110" s="70"/>
       <c r="L110" s="83" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M110" s="70"/>
       <c r="N110" s="83" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O110" s="70"/>
       <c r="P110" s="70" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q110" s="70"/>
       <c r="R110" s="70"/>
@@ -5604,13 +5604,13 @@
         <v>71</v>
       </c>
       <c r="B111" s="70" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C111" s="70" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D111" s="70" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E111" s="70"/>
       <c r="F111" s="70"/>
@@ -5620,15 +5620,15 @@
       <c r="J111" s="70"/>
       <c r="K111" s="70"/>
       <c r="L111" s="83" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M111" s="70"/>
       <c r="N111" s="83" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O111" s="70"/>
       <c r="P111" s="70" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q111" s="70"/>
       <c r="R111" s="70"/>
@@ -5647,16 +5647,16 @@
         <v>70</v>
       </c>
       <c r="B112" s="70" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C112" s="70" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D112" s="70" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E112" s="70" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F112" s="70"/>
       <c r="G112" s="70"/>
@@ -5665,15 +5665,15 @@
       <c r="J112" s="70"/>
       <c r="K112" s="70"/>
       <c r="L112" s="83" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M112" s="70"/>
       <c r="N112" s="83" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O112" s="70"/>
       <c r="P112" s="70" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q112" s="70"/>
       <c r="R112" s="70"/>
@@ -5690,16 +5690,16 @@
         <v>70</v>
       </c>
       <c r="B113" s="15" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C113" s="15" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D113" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E113" s="15" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F113" s="15"/>
       <c r="G113" s="15"/>
@@ -5708,15 +5708,15 @@
       <c r="J113" s="15"/>
       <c r="K113" s="15"/>
       <c r="L113" s="58" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M113" s="15"/>
       <c r="N113" s="58" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O113" s="15"/>
       <c r="P113" s="15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q113" s="15"/>
       <c r="R113" s="15"/>
@@ -5733,13 +5733,13 @@
         <v>71</v>
       </c>
       <c r="B114" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="C114" s="15" t="s">
         <v>237</v>
       </c>
-      <c r="C114" s="15" t="s">
-        <v>239</v>
-      </c>
       <c r="D114" s="15" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E114" s="15"/>
       <c r="F114" s="15"/>
@@ -5749,15 +5749,15 @@
       <c r="J114" s="15"/>
       <c r="K114" s="15"/>
       <c r="L114" s="58" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M114" s="15"/>
       <c r="N114" s="58" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O114" s="15"/>
       <c r="P114" s="15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q114" s="15"/>
       <c r="R114" s="15"/>
@@ -5776,16 +5776,16 @@
         <v>70</v>
       </c>
       <c r="B115" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="C115" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="D115" s="15" t="s">
         <v>238</v>
       </c>
-      <c r="C115" s="15" t="s">
-        <v>239</v>
-      </c>
-      <c r="D115" s="15" t="s">
-        <v>240</v>
-      </c>
       <c r="E115" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F115" s="15"/>
       <c r="G115" s="15"/>
@@ -5794,15 +5794,15 @@
       <c r="J115" s="15"/>
       <c r="K115" s="15"/>
       <c r="L115" s="58" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M115" s="15"/>
       <c r="N115" s="58" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O115" s="15"/>
       <c r="P115" s="15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q115" s="15"/>
       <c r="R115" s="15"/>
@@ -5819,16 +5819,16 @@
         <v>70</v>
       </c>
       <c r="B116" s="13" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C116" s="13" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D116" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E116" s="13" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F116" s="13"/>
       <c r="G116" s="13"/>
@@ -5837,15 +5837,15 @@
       <c r="J116" s="13"/>
       <c r="K116" s="13"/>
       <c r="L116" s="56" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M116" s="13"/>
       <c r="N116" s="56" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O116" s="13"/>
       <c r="P116" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q116" s="13"/>
       <c r="R116" s="13"/>
@@ -5862,13 +5862,13 @@
         <v>71</v>
       </c>
       <c r="B117" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="C117" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="C117" s="13" t="s">
-        <v>201</v>
-      </c>
       <c r="D117" s="13" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E117" s="13"/>
       <c r="F117" s="13"/>
@@ -5878,15 +5878,15 @@
       <c r="J117" s="13"/>
       <c r="K117" s="13"/>
       <c r="L117" s="56" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M117" s="13"/>
       <c r="N117" s="56" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O117" s="13"/>
       <c r="P117" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q117" s="13"/>
       <c r="R117" s="13"/>
@@ -5905,16 +5905,16 @@
         <v>70</v>
       </c>
       <c r="B118" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="C118" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="D118" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="C118" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="D118" s="13" t="s">
-        <v>202</v>
-      </c>
       <c r="E118" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F118" s="13"/>
       <c r="G118" s="13"/>
@@ -5923,15 +5923,15 @@
       <c r="J118" s="13"/>
       <c r="K118" s="13"/>
       <c r="L118" s="56" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M118" s="13"/>
       <c r="N118" s="56" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O118" s="13"/>
       <c r="P118" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q118" s="13"/>
       <c r="R118" s="13"/>
@@ -5968,22 +5968,22 @@
     </row>
     <row r="126" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="127" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="128" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="130" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A130" s="37" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E130" s="36"/>
       <c r="F130" s="36"/>
@@ -6044,10 +6044,10 @@
     <row r="134" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A134" s="37"/>
       <c r="B134" s="38" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C134" s="68" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E134" s="36"/>
       <c r="F134" s="36"/>
@@ -6064,7 +6064,7 @@
       <c r="A135" s="37"/>
       <c r="B135" s="38"/>
       <c r="C135" s="79" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E135" s="36"/>
       <c r="F135" s="36"/>
@@ -6095,10 +6095,10 @@
     <row r="137" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A137" s="37"/>
       <c r="B137" s="38" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C137" s="86" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E137" s="36"/>
       <c r="F137" s="36"/>
@@ -6115,7 +6115,7 @@
       <c r="A138" s="37"/>
       <c r="B138" s="38"/>
       <c r="C138" s="79" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E138" s="36"/>
       <c r="F138" s="36"/>
@@ -6153,10 +6153,10 @@
     <row r="140" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A140" s="37"/>
       <c r="B140" s="38" t="s">
+        <v>131</v>
+      </c>
+      <c r="C140" t="s">
         <v>133</v>
-      </c>
-      <c r="C140" t="s">
-        <v>135</v>
       </c>
       <c r="E140" s="36"/>
       <c r="F140" s="36"/>
@@ -6173,7 +6173,7 @@
       <c r="A141" s="37"/>
       <c r="B141" s="38"/>
       <c r="C141" s="65" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E141" s="36"/>
       <c r="F141" s="36"/>
@@ -6204,10 +6204,10 @@
     <row r="143" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A143" s="37"/>
       <c r="B143" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="C143" s="86" t="s">
         <v>163</v>
-      </c>
-      <c r="C143" s="86" t="s">
-        <v>165</v>
       </c>
       <c r="E143" s="36"/>
       <c r="F143" s="36"/>
@@ -6224,7 +6224,7 @@
       <c r="A144" s="37"/>
       <c r="B144" s="38"/>
       <c r="C144" s="65" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E144" s="36"/>
       <c r="F144" s="36"/>
@@ -6253,10 +6253,10 @@
     <row r="146" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A146" s="37"/>
       <c r="B146" s="38" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C146" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F146" s="36"/>
       <c r="G146" s="36"/>
@@ -6272,7 +6272,7 @@
       <c r="A147" s="37"/>
       <c r="B147" s="38"/>
       <c r="C147" s="39" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F147" s="36"/>
       <c r="G147" s="36"/>
@@ -6315,7 +6315,7 @@
     <row r="150" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A150" s="37"/>
       <c r="B150" s="42" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C150" s="43">
         <v>1.1399999999999999</v>
@@ -6339,7 +6339,7 @@
     <row r="151" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A151" s="37"/>
       <c r="B151" s="46" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C151" s="45">
         <v>7.0000000000000007E-2</v>
@@ -6374,13 +6374,13 @@
         <v>Fixed O&amp;M cost [€/MWyear]</v>
       </c>
       <c r="E152" s="47" t="s">
+        <v>114</v>
+      </c>
+      <c r="F152" s="47" t="s">
+        <v>115</v>
+      </c>
+      <c r="G152" s="47" t="s">
         <v>116</v>
-      </c>
-      <c r="F152" s="47" t="s">
-        <v>117</v>
-      </c>
-      <c r="G152" s="47" t="s">
-        <v>118</v>
       </c>
       <c r="H152" s="49" t="str">
         <f xml:space="preserve"> "Annual fixed costs [" &amp;B43 &amp; "/year]"</f>
@@ -6395,27 +6395,27 @@
         <v>Fuel cost [€/MWh]</v>
       </c>
       <c r="K152" s="46" t="s">
+        <v>117</v>
+      </c>
+      <c r="L152" s="46" t="s">
+        <v>118</v>
+      </c>
+      <c r="M152" s="48" t="s">
         <v>119</v>
-      </c>
-      <c r="L152" s="46" t="s">
-        <v>120</v>
-      </c>
-      <c r="M152" s="48" t="s">
-        <v>121</v>
       </c>
       <c r="N152" s="47"/>
       <c r="O152" s="47"/>
       <c r="P152" s="48" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Q152" s="88" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="R152" s="87"/>
     </row>
     <row r="153" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B153" s="45" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C153" s="50">
         <f>103100</f>
@@ -6456,7 +6456,7 @@
     </row>
     <row r="154" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B154" s="51" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C154" s="45">
         <f>1612000</f>
@@ -6523,7 +6523,7 @@
     </row>
     <row r="156" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B156" s="51" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C156" s="45">
         <v>1969000</v>
@@ -6571,7 +6571,7 @@
     </row>
     <row r="157" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B157" s="45" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C157" s="45"/>
       <c r="D157" s="45"/>
@@ -6654,7 +6654,7 @@
     </row>
     <row r="160" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B160" s="45" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C160" s="45">
         <v>5580000</v>
@@ -6695,7 +6695,7 @@
         <v>-1.22</v>
       </c>
       <c r="R160" s="87" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="161" spans="2:18" x14ac:dyDescent="0.2">
@@ -6719,7 +6719,7 @@
     </row>
     <row r="162" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B162" s="45" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C162" s="45"/>
       <c r="D162" s="45"/>
@@ -6743,7 +6743,7 @@
     </row>
     <row r="163" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B163" s="45" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C163" s="45"/>
       <c r="D163" s="45"/>
@@ -6767,7 +6767,7 @@
     </row>
     <row r="165" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B165" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="167" spans="2:18" x14ac:dyDescent="0.2">

</xml_diff>